<commit_message>
updated output for species ID
</commit_message>
<xml_diff>
--- a/data/sequencing_metabolomics_samples.xlsx
+++ b/data/sequencing_metabolomics_samples.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashuffmyer/MyProjects/moorea_symbiotic_exchange_2023/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4AAE880-361F-AF41-9E93-374B458EC42D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2679E5F7-82CB-DA46-9052-2FF1FE266FF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33500" yWindow="680" windowWidth="32920" windowHeight="16720" xr2:uid="{0E9B6F04-84CF-7349-B5EA-1343C1B06CB7}"/>
+    <workbookView xWindow="-37580" yWindow="-1460" windowWidth="19120" windowHeight="19260" xr2:uid="{0E9B6F04-84CF-7349-B5EA-1343C1B06CB7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="64">
   <si>
     <t>RNA</t>
   </si>
@@ -129,6 +129,105 @@
   </si>
   <si>
     <t>2 adult/recruit dark; 3 larvae dark</t>
+  </si>
+  <si>
+    <t>Previous metabolomics w/ Rutgers</t>
+  </si>
+  <si>
+    <t>1484 total / 28 samples</t>
+  </si>
+  <si>
+    <t>OPTION 4: POC vs ACR RNA and Metabolomics</t>
+  </si>
+  <si>
+    <t>OPTION 2: All species metabolomics</t>
+  </si>
+  <si>
+    <t>OPTION 3: POC RNA and Metabolomics</t>
+  </si>
+  <si>
+    <t>OPTION 1: POC vs ACR RNA</t>
+  </si>
+  <si>
+    <t>POC and ACR RNA and metabolomics</t>
+  </si>
+  <si>
+    <t>n=6 per sample</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RNA: TagSeq or RNAseq? </t>
+  </si>
+  <si>
+    <t>Pending quotes</t>
+  </si>
+  <si>
+    <t>n=4 per species</t>
+  </si>
+  <si>
+    <t>Dark Controls</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Could do this if we didn't use all of domestic travel or operating charges </t>
+  </si>
+  <si>
+    <t>$163 per sample for Standard PolyA RNAseq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Excess on another grant? </t>
+  </si>
+  <si>
+    <t>Still need final bill for ITS2 as well</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$53 per sample from previous work </t>
+  </si>
+  <si>
+    <t>PREFERRED OPTION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oklahoma sequencing </t>
+  </si>
+  <si>
+    <t>Submit on Genohub</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30M depth </t>
+  </si>
+  <si>
+    <t>PolyA selection</t>
+  </si>
+  <si>
+    <t>150bp</t>
+  </si>
+  <si>
+    <t>Standard RNAseq</t>
+  </si>
+  <si>
+    <t>Okalhoma Medical Reseach Foundation NGS core</t>
+  </si>
+  <si>
+    <t>mixed species to get n=6 per</t>
+  </si>
+  <si>
+    <t>A. hya/A. ret  recruit</t>
+  </si>
+  <si>
+    <t>n=5-6 per treatment</t>
+  </si>
+  <si>
+    <t>A. spp mix  recruit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Submitted genohub for 64 samples </t>
+  </si>
+  <si>
+    <t>30M reads minimum per sample</t>
+  </si>
+  <si>
+    <t>Library prep + sequencing</t>
+  </si>
+  <si>
+    <t>n=6  from P. mea larvae at 27C (DNA)</t>
   </si>
 </sst>
 </file>
@@ -151,7 +250,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -161,6 +260,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -257,25 +380,32 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -610,33 +740,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB2E6D95-23B3-7347-9DA6-89D7D1C793C1}">
-  <dimension ref="D2:W29"/>
+  <dimension ref="D2:W48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="T18" sqref="T18"/>
+    <sheetView tabSelected="1" topLeftCell="C8" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="27.1640625" customWidth="1"/>
+    <col min="4" max="4" width="37.6640625" customWidth="1"/>
     <col min="7" max="7" width="15.33203125" customWidth="1"/>
-    <col min="9" max="9" width="18.33203125" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" customWidth="1"/>
+    <col min="9" max="9" width="25" customWidth="1"/>
+    <col min="10" max="10" width="18.6640625" customWidth="1"/>
     <col min="11" max="11" width="18.5" customWidth="1"/>
-    <col min="12" max="12" width="15.1640625" customWidth="1"/>
+    <col min="12" max="12" width="19.6640625" customWidth="1"/>
     <col min="16" max="16" width="16.1640625" customWidth="1"/>
     <col min="18" max="18" width="23.1640625" customWidth="1"/>
     <col min="19" max="19" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="4:23" x14ac:dyDescent="0.2">
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="K2">
-        <v>2</v>
-      </c>
-      <c r="P2">
-        <v>3</v>
+      <c r="G2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="4:23" x14ac:dyDescent="0.2">
@@ -666,377 +798,616 @@
       <c r="G4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="6"/>
-      <c r="I4" s="7"/>
+      <c r="I4" s="6"/>
       <c r="K4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="7"/>
+      <c r="N4" s="6"/>
       <c r="P4" s="5"/>
-      <c r="Q4" s="6"/>
-      <c r="R4" s="6"/>
-      <c r="S4" s="6"/>
-      <c r="T4" s="6"/>
-      <c r="U4" s="6"/>
-      <c r="V4" s="6"/>
-      <c r="W4" s="7"/>
+      <c r="W4" s="6"/>
     </row>
     <row r="5" spans="4:23" x14ac:dyDescent="0.2">
       <c r="G5" s="5"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="7"/>
+      <c r="I5" s="6"/>
       <c r="K5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="L5" s="6" t="s">
+      <c r="L5" t="s">
         <v>4</v>
       </c>
-      <c r="M5" s="6">
+      <c r="M5">
         <v>15</v>
       </c>
-      <c r="N5" s="7"/>
-      <c r="P5" s="8" t="s">
+      <c r="N5" s="6"/>
+      <c r="P5" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="Q5" s="6"/>
-      <c r="R5" s="6"/>
-      <c r="S5" s="9" t="s">
+      <c r="S5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="T5" s="6"/>
-      <c r="U5" s="6"/>
-      <c r="V5" s="6"/>
-      <c r="W5" s="7"/>
+      <c r="W5" s="6"/>
     </row>
     <row r="6" spans="4:23" x14ac:dyDescent="0.2">
       <c r="G6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6">
         <v>18</v>
       </c>
-      <c r="I6" s="7" t="s">
+      <c r="I6" s="6" t="s">
         <v>19</v>
       </c>
       <c r="K6" s="5"/>
-      <c r="L6" s="6" t="s">
+      <c r="L6" t="s">
         <v>5</v>
       </c>
-      <c r="M6" s="6">
+      <c r="M6">
         <v>15</v>
       </c>
-      <c r="N6" s="7"/>
+      <c r="N6" s="6"/>
       <c r="P6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="Q6" s="6">
+      <c r="Q6">
         <v>10</v>
       </c>
-      <c r="R6" s="6" t="s">
+      <c r="R6" t="s">
         <v>20</v>
       </c>
-      <c r="S6" s="6" t="s">
+      <c r="S6" t="s">
         <v>21</v>
       </c>
-      <c r="T6" s="6">
+      <c r="T6">
         <v>15</v>
       </c>
-      <c r="U6" s="6" t="s">
+      <c r="U6" t="s">
         <v>22</v>
       </c>
-      <c r="V6" s="6"/>
-      <c r="W6" s="7"/>
+      <c r="W6" s="6"/>
     </row>
     <row r="7" spans="4:23" x14ac:dyDescent="0.2">
       <c r="G7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7">
         <v>18</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="I7" s="6" t="s">
         <v>19</v>
       </c>
       <c r="K7" s="5"/>
-      <c r="L7" s="6" t="s">
+      <c r="L7" t="s">
         <v>6</v>
       </c>
-      <c r="M7" s="6">
+      <c r="M7">
         <v>15</v>
       </c>
-      <c r="N7" s="7"/>
+      <c r="N7" s="6"/>
       <c r="P7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="Q7" s="6">
+      <c r="Q7">
         <v>18</v>
       </c>
-      <c r="R7" s="6" t="s">
+      <c r="R7" t="s">
         <v>23</v>
       </c>
-      <c r="S7" s="6" t="s">
+      <c r="S7" t="s">
         <v>17</v>
       </c>
-      <c r="T7" s="6">
+      <c r="T7">
         <v>18</v>
       </c>
-      <c r="U7" s="6" t="s">
+      <c r="U7" t="s">
         <v>23</v>
       </c>
-      <c r="V7" s="6"/>
-      <c r="W7" s="7"/>
+      <c r="W7" s="6"/>
     </row>
     <row r="8" spans="4:23" x14ac:dyDescent="0.2">
       <c r="G8" s="5"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="7"/>
+      <c r="I8" s="6"/>
       <c r="K8" s="5"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="7"/>
+      <c r="N8" s="6"/>
       <c r="P8" s="5"/>
-      <c r="Q8" s="6"/>
-      <c r="R8" s="6"/>
-      <c r="S8" s="17" t="s">
+      <c r="S8" t="s">
         <v>29</v>
       </c>
-      <c r="T8" s="6">
+      <c r="T8">
         <v>5</v>
       </c>
-      <c r="U8" s="6" t="s">
+      <c r="U8" t="s">
         <v>30</v>
       </c>
-      <c r="V8" s="6"/>
-      <c r="W8" s="7"/>
+      <c r="W8" s="6"/>
     </row>
     <row r="9" spans="4:23" x14ac:dyDescent="0.2">
       <c r="G9" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="H9" s="6">
+      <c r="H9">
         <v>10</v>
       </c>
-      <c r="I9" s="7" t="s">
+      <c r="I9" s="6" t="s">
         <v>20</v>
       </c>
       <c r="K9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="L9" s="6" t="s">
+      <c r="L9" t="s">
         <v>4</v>
       </c>
-      <c r="M9" s="6">
+      <c r="M9">
         <v>21</v>
       </c>
-      <c r="N9" s="7"/>
+      <c r="N9" s="6"/>
       <c r="P9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="Q9" s="6">
+      <c r="Q9">
         <f>SUM(Q6,Q7)</f>
         <v>28</v>
       </c>
-      <c r="R9" s="6"/>
-      <c r="S9" s="6" t="s">
+      <c r="S9" t="s">
         <v>15</v>
       </c>
-      <c r="T9" s="6">
+      <c r="T9">
         <f>SUM(T6,T7,T8)</f>
         <v>38</v>
       </c>
-      <c r="U9" s="6"/>
-      <c r="V9" s="6"/>
-      <c r="W9" s="7"/>
+      <c r="W9" s="6"/>
     </row>
     <row r="10" spans="4:23" x14ac:dyDescent="0.2">
       <c r="G10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="6">
+      <c r="H10" s="24">
         <v>18</v>
       </c>
-      <c r="I10" s="7"/>
+      <c r="I10" s="23" t="s">
+        <v>56</v>
+      </c>
       <c r="K10" s="5"/>
-      <c r="L10" s="6" t="s">
+      <c r="L10" t="s">
         <v>5</v>
       </c>
-      <c r="M10" s="6">
+      <c r="M10">
         <v>21</v>
       </c>
-      <c r="N10" s="7"/>
+      <c r="N10" s="6"/>
       <c r="P10" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="Q10" s="11">
-        <v>160</v>
-      </c>
-      <c r="R10" s="6"/>
-      <c r="S10" s="6" t="s">
+      <c r="Q10" s="9">
+        <v>163</v>
+      </c>
+      <c r="S10" t="s">
         <v>14</v>
       </c>
-      <c r="T10" s="11">
-        <v>120</v>
-      </c>
-      <c r="U10" s="6"/>
-      <c r="V10" s="6"/>
-      <c r="W10" s="7"/>
+      <c r="T10" s="9">
+        <v>53</v>
+      </c>
+      <c r="W10" s="6"/>
     </row>
     <row r="11" spans="4:23" x14ac:dyDescent="0.2">
       <c r="G11" s="5"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="7"/>
+      <c r="I11" s="6"/>
       <c r="K11" s="5"/>
-      <c r="L11" s="6" t="s">
+      <c r="L11" t="s">
         <v>6</v>
       </c>
-      <c r="M11" s="6">
+      <c r="M11">
         <v>21</v>
       </c>
-      <c r="N11" s="7"/>
-      <c r="P11" s="8" t="s">
+      <c r="N11" s="6"/>
+      <c r="P11" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="Q11" s="9">
+      <c r="Q11" s="1">
         <f>Q10*Q9</f>
-        <v>4480</v>
-      </c>
-      <c r="R11" s="6"/>
-      <c r="S11" s="9" t="s">
+        <v>4564</v>
+      </c>
+      <c r="S11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="T11" s="9">
+      <c r="T11" s="1">
         <f>T10*T9</f>
-        <v>4560</v>
-      </c>
-      <c r="U11" s="6"/>
-      <c r="V11" s="6"/>
-      <c r="W11" s="7"/>
+        <v>2014</v>
+      </c>
+      <c r="W11" s="6"/>
     </row>
     <row r="12" spans="4:23" x14ac:dyDescent="0.2">
-      <c r="G12" s="8" t="s">
+      <c r="G12" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H12" s="9">
+      <c r="H12" s="1">
         <f>SUM(H6:H10)</f>
         <v>64</v>
       </c>
-      <c r="I12" s="10"/>
+      <c r="I12" s="8"/>
       <c r="K12" s="5"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="7"/>
+      <c r="N12" s="6"/>
       <c r="P12" s="5"/>
-      <c r="Q12" s="6"/>
-      <c r="R12" s="6"/>
-      <c r="S12" s="6"/>
-      <c r="T12" s="6"/>
-      <c r="U12" s="6"/>
-      <c r="V12" s="6"/>
-      <c r="W12" s="7"/>
+      <c r="W12" s="6"/>
     </row>
     <row r="13" spans="4:23" x14ac:dyDescent="0.2">
       <c r="G13" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H13" s="11">
-        <v>160</v>
-      </c>
-      <c r="I13" s="7"/>
+      <c r="H13" s="9">
+        <v>163</v>
+      </c>
+      <c r="I13" s="6"/>
       <c r="K13" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="L13" s="6" t="s">
+      <c r="L13" t="s">
         <v>9</v>
       </c>
-      <c r="M13" s="6">
+      <c r="M13">
         <v>21</v>
       </c>
-      <c r="N13" s="7"/>
-      <c r="P13" s="12" t="s">
+      <c r="N13" s="6"/>
+      <c r="P13" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="Q13" s="13">
+      <c r="Q13" s="19">
         <f>Q11+T11</f>
-        <v>9040</v>
-      </c>
-      <c r="R13" s="16"/>
-      <c r="S13" s="16"/>
-      <c r="T13" s="16"/>
-      <c r="U13" s="16"/>
-      <c r="V13" s="16"/>
-      <c r="W13" s="14"/>
+        <v>6578</v>
+      </c>
+      <c r="R13" s="14"/>
+      <c r="S13" s="14"/>
+      <c r="T13" s="14"/>
+      <c r="U13" s="14"/>
+      <c r="V13" s="14"/>
+      <c r="W13" s="12"/>
     </row>
     <row r="14" spans="4:23" x14ac:dyDescent="0.2">
       <c r="G14" s="5"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="7"/>
+      <c r="I14" s="6"/>
       <c r="K14" s="5"/>
-      <c r="L14" s="6"/>
-      <c r="M14" s="6"/>
-      <c r="N14" s="7"/>
+      <c r="N14" s="6"/>
     </row>
     <row r="15" spans="4:23" x14ac:dyDescent="0.2">
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="G15" s="12" t="s">
+      <c r="G15" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="H15" s="13">
+      <c r="H15" s="19">
         <f>H13*H12</f>
-        <v>10240</v>
-      </c>
-      <c r="I15" s="14"/>
+        <v>10432</v>
+      </c>
+      <c r="I15" s="12"/>
       <c r="K15" s="5"/>
-      <c r="L15" s="9" t="s">
+      <c r="L15" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M15" s="9">
+      <c r="M15" s="1">
         <f>SUM(M5:M13)</f>
         <v>129</v>
       </c>
-      <c r="N15" s="7"/>
+      <c r="N15" s="6"/>
     </row>
     <row r="16" spans="4:23" x14ac:dyDescent="0.2">
-      <c r="D16">
-        <v>10551</v>
+      <c r="D16" s="18">
+        <v>10600</v>
       </c>
       <c r="K16" s="5"/>
-      <c r="L16" s="6" t="s">
+      <c r="L16" t="s">
         <v>14</v>
       </c>
-      <c r="M16" s="11">
-        <v>120</v>
-      </c>
-      <c r="N16" s="7"/>
+      <c r="M16" s="9">
+        <v>53</v>
+      </c>
+      <c r="N16" s="6"/>
     </row>
     <row r="17" spans="4:14" x14ac:dyDescent="0.2">
       <c r="K17" s="5"/>
-      <c r="L17" s="6"/>
-      <c r="M17" s="6"/>
-      <c r="N17" s="7"/>
+      <c r="N17" s="6"/>
     </row>
     <row r="18" spans="4:14" x14ac:dyDescent="0.2">
-      <c r="K18" s="15"/>
-      <c r="L18" s="13" t="s">
+      <c r="K18" s="13"/>
+      <c r="L18" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="M18" s="13">
+      <c r="M18" s="19">
         <f>M16*M15</f>
-        <v>15480</v>
-      </c>
-      <c r="N18" s="14"/>
+        <v>6837</v>
+      </c>
+      <c r="N18" s="12"/>
     </row>
     <row r="19" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D19" s="1"/>
     </row>
+    <row r="20" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="D20" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" s="9"/>
+    </row>
+    <row r="21" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="D21" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E21" s="9"/>
+    </row>
+    <row r="22" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="D22" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E22" s="9"/>
+      <c r="G22" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="G23" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="4"/>
+    </row>
     <row r="24" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D24" s="1"/>
+      <c r="G24" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H24" s="15"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="15"/>
+      <c r="K24" s="15"/>
+      <c r="L24" s="6"/>
+    </row>
+    <row r="25" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="G25" s="5"/>
+      <c r="H25" s="15"/>
+      <c r="I25" s="15"/>
+      <c r="J25" s="15"/>
+      <c r="K25" s="15"/>
+      <c r="L25" s="6"/>
+    </row>
+    <row r="26" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="D26" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="H26" s="15"/>
+      <c r="J26" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="K26" s="15"/>
+      <c r="L26" s="6"/>
+    </row>
+    <row r="27" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="D27" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H27" s="15">
+        <v>10</v>
+      </c>
+      <c r="I27" t="s">
+        <v>20</v>
+      </c>
+      <c r="J27" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="K27" s="15">
+        <v>15</v>
+      </c>
+      <c r="L27" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="D28" t="s">
+        <v>44</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H28" s="15">
+        <v>18</v>
+      </c>
+      <c r="I28" t="s">
+        <v>23</v>
+      </c>
+      <c r="J28" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="K28" s="15">
+        <v>18</v>
+      </c>
+      <c r="L28" s="6" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="29" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D29" s="1"/>
+      <c r="G29" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="H29" s="24">
+        <v>18</v>
+      </c>
+      <c r="I29" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="J29" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="K29" s="22">
+        <v>16</v>
+      </c>
+      <c r="L29" s="23" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="G30" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H30" s="15">
+        <v>18</v>
+      </c>
+      <c r="I30" t="s">
+        <v>23</v>
+      </c>
+      <c r="J30" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="K30" s="15">
+        <v>8</v>
+      </c>
+      <c r="L30" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="31" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="D31" s="1"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="15"/>
+      <c r="J31" s="15"/>
+      <c r="K31" s="15"/>
+      <c r="L31" s="6"/>
+    </row>
+    <row r="32" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="D32" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="G32" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H32" s="16">
+        <f>SUM(H27:H30)</f>
+        <v>64</v>
+      </c>
+      <c r="J32" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="K32" s="16">
+        <f>SUM(K27:K30)</f>
+        <v>57</v>
+      </c>
+      <c r="L32" s="6"/>
+    </row>
+    <row r="33" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="D33" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H33" s="15">
+        <v>163</v>
+      </c>
+      <c r="J33" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="K33" s="15">
+        <v>53</v>
+      </c>
+      <c r="L33" s="6"/>
+    </row>
+    <row r="34" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="G34" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H34" s="15">
+        <f>H32*H33</f>
+        <v>10432</v>
+      </c>
+      <c r="J34" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="K34" s="15">
+        <f>K33*K32</f>
+        <v>3021</v>
+      </c>
+      <c r="L34" s="6"/>
+    </row>
+    <row r="35" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="G35" s="5"/>
+      <c r="H35" s="15"/>
+      <c r="I35" s="15"/>
+      <c r="J35" s="15"/>
+      <c r="K35" s="15"/>
+      <c r="L35" s="6"/>
+    </row>
+    <row r="36" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="G36" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="H36" s="20">
+        <f>SUM(H34,K34)</f>
+        <v>13453</v>
+      </c>
+      <c r="I36" s="14"/>
+      <c r="J36" s="14"/>
+      <c r="K36" s="14"/>
+      <c r="L36" s="12"/>
+    </row>
+    <row r="38" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="H38" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="39" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="H39" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="41" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="G41" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="43" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="G43" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J43" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="44" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="G44" t="s">
+        <v>51</v>
+      </c>
+      <c r="J44" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="45" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="G45" t="s">
+        <v>52</v>
+      </c>
+      <c r="J45" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="46" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="G46" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="47" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="G47" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="48" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="G48" t="s">
+        <v>55</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>